<commit_message>
Stand DM nach Transfer von Daten
</commit_message>
<xml_diff>
--- a/doc/20220103_Kopie_DM faults_de_frz_en.xlsx
+++ b/doc/20220103_Kopie_DM faults_de_frz_en.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13050" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Grundlegende Attribute" sheetId="2" r:id="rId1"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="422">
   <si>
     <t>Grundlegende Attribute</t>
   </si>
@@ -1837,6 +1837,9 @@
   </si>
   <si>
     <t>effacé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in Datenbank nicht auf MANDATORY gesetzt </t>
   </si>
 </sst>
 </file>
@@ -2847,7 +2850,7 @@
     <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="294">
+  <cellXfs count="292">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3254,9 +3257,6 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3301,9 +3301,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3374,12 +3371,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3391,9 +3382,6 @@
     <xf numFmtId="0" fontId="19" fillId="13" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3656,6 +3644,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4049,8 +4046,8 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>414032</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>153471</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>62757</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4863,8 +4860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG35"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4912,10 +4909,10 @@
       <c r="H6" s="11"/>
     </row>
     <row r="8" spans="1:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="252" t="s">
+      <c r="A8" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="247"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="61"/>
@@ -4932,10 +4929,10 @@
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="254" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="259"/>
+      <c r="B10" s="254"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -4978,7 +4975,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="39" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="260" t="s">
+      <c r="A13" s="255" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -5002,7 +4999,7 @@
       <c r="H13" s="139"/>
     </row>
     <row r="14" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="250"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="10" t="s">
         <v>7</v>
       </c>
@@ -5022,7 +5019,7 @@
       <c r="H14" s="140"/>
     </row>
     <row r="15" spans="1:8" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="250"/>
+      <c r="A15" s="245"/>
       <c r="B15" s="10" t="s">
         <v>9</v>
       </c>
@@ -5046,7 +5043,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="261"/>
+      <c r="A16" s="256"/>
       <c r="B16" s="33" t="s">
         <v>10</v>
       </c>
@@ -5070,7 +5067,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="253" t="s">
+      <c r="A17" s="248" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="32" t="s">
@@ -5092,7 +5089,7 @@
       <c r="H17" s="139"/>
     </row>
     <row r="18" spans="1:33" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="254"/>
+      <c r="A18" s="249"/>
       <c r="B18" s="10" t="s">
         <v>12</v>
       </c>
@@ -5112,11 +5109,11 @@
       <c r="H18" s="139"/>
     </row>
     <row r="19" spans="1:33" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="255"/>
+      <c r="A19" s="250"/>
       <c r="B19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="149" t="s">
+      <c r="C19" s="148" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="26" t="s">
@@ -5132,7 +5129,7 @@
       <c r="H19" s="139"/>
     </row>
     <row r="20" spans="1:33" ht="102.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="256" t="s">
+      <c r="A20" s="251" t="s">
         <v>3</v>
       </c>
       <c r="B20" s="38" t="s">
@@ -5156,7 +5153,7 @@
       <c r="H20" s="139"/>
     </row>
     <row r="21" spans="1:33" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="254"/>
+      <c r="A21" s="249"/>
       <c r="B21" s="10" t="s">
         <v>15</v>
       </c>
@@ -5178,7 +5175,7 @@
       </c>
     </row>
     <row r="22" spans="1:33" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="255"/>
+      <c r="A22" s="250"/>
       <c r="B22" s="36" t="s">
         <v>16</v>
       </c>
@@ -5198,7 +5195,7 @@
       </c>
     </row>
     <row r="23" spans="1:33" ht="161.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="257" t="s">
+      <c r="A23" s="252" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="30" t="s">
@@ -5220,7 +5217,7 @@
       <c r="H23" s="143"/>
     </row>
     <row r="24" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A24" s="254"/>
+      <c r="A24" s="249"/>
       <c r="B24" s="10" t="s">
         <v>172</v>
       </c>
@@ -5236,7 +5233,7 @@
       <c r="F24" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="G24" s="227" t="s">
+      <c r="G24" s="222" t="s">
         <v>221</v>
       </c>
       <c r="H24" s="144" t="s">
@@ -5244,7 +5241,7 @@
       </c>
     </row>
     <row r="25" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="254"/>
+      <c r="A25" s="249"/>
       <c r="B25" s="27" t="s">
         <v>196</v>
       </c>
@@ -5266,7 +5263,7 @@
       </c>
     </row>
     <row r="26" spans="1:33" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="254"/>
+      <c r="A26" s="249"/>
       <c r="B26" s="27" t="s">
         <v>197</v>
       </c>
@@ -5283,12 +5280,12 @@
         <v>199</v>
       </c>
       <c r="G26" s="46"/>
-      <c r="H26" s="206" t="s">
+      <c r="H26" s="201" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:33" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="254"/>
+      <c r="A27" s="249"/>
       <c r="B27" s="63" t="s">
         <v>170</v>
       </c>
@@ -5312,7 +5309,7 @@
       </c>
     </row>
     <row r="28" spans="1:33" ht="266.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="258"/>
+      <c r="A28" s="253"/>
       <c r="B28" s="41" t="s">
         <v>18</v>
       </c>
@@ -5343,51 +5340,53 @@
       <c r="AG28" s="4"/>
     </row>
     <row r="29" spans="1:33" ht="26.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="249" t="s">
+      <c r="A29" s="244" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="63" t="s">
+      <c r="D29" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="63" t="s">
+      <c r="E29" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="F29" s="63" t="s">
+      <c r="F29" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="G29" s="63"/>
-      <c r="H29" s="177" t="s">
+      <c r="G29" s="10"/>
+      <c r="H29" s="175" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="30" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="250"/>
-      <c r="B30" s="63" t="s">
+      <c r="A30" s="245"/>
+      <c r="B30" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="290" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="63" t="s">
+      <c r="D30" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="63" t="s">
+      <c r="E30" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="F30" s="63" t="s">
+      <c r="F30" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G30" s="63"/>
-      <c r="H30" s="146"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="291" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="31" spans="1:33" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="251"/>
+      <c r="A31" s="246"/>
       <c r="B31" s="63" t="s">
         <v>20</v>
       </c>
@@ -5443,8 +5442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG73"/>
   <sheetViews>
-    <sheetView zoomScale="63" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A22" zoomScale="63" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5493,10 +5492,10 @@
       <c r="I6" s="11"/>
     </row>
     <row r="8" spans="1:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="252" t="s">
+      <c r="A8" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="247"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
@@ -5513,11 +5512,11 @@
       <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="254" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="259"/>
-      <c r="C10" s="259"/>
+      <c r="B10" s="254"/>
+      <c r="C10" s="254"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
@@ -5535,23 +5534,23 @@
       <c r="H11" s="17"/>
     </row>
     <row r="12" spans="1:9" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="230"/>
-      <c r="C12" s="231" t="s">
+      <c r="B12" s="225"/>
+      <c r="C12" s="226" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="231" t="s">
+      <c r="D12" s="226" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="231" t="s">
+      <c r="E12" s="226" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="231" t="s">
+      <c r="F12" s="226" t="s">
         <v>211</v>
       </c>
-      <c r="G12" s="231" t="s">
+      <c r="G12" s="226" t="s">
         <v>188</v>
       </c>
-      <c r="H12" s="231" t="s">
+      <c r="H12" s="226" t="s">
         <v>190</v>
       </c>
       <c r="I12" s="138" t="s">
@@ -5559,71 +5558,71 @@
       </c>
     </row>
     <row r="13" spans="1:9" s="9" customFormat="1" ht="15.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="272" t="s">
+      <c r="B13" s="267" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="240" t="s">
+      <c r="C13" s="235" t="s">
         <v>399</v>
       </c>
-      <c r="D13" s="232" t="s">
+      <c r="D13" s="227" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="233" t="s">
+      <c r="E13" s="228" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="233" t="s">
+      <c r="F13" s="228" t="s">
         <v>215</v>
       </c>
-      <c r="G13" s="240" t="s">
+      <c r="G13" s="235" t="s">
         <v>402</v>
       </c>
-      <c r="H13" s="241"/>
-      <c r="I13" s="239"/>
+      <c r="H13" s="236"/>
+      <c r="I13" s="234"/>
     </row>
     <row r="14" spans="1:9" s="9" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="272"/>
-      <c r="C14" s="238" t="s">
+      <c r="B14" s="267"/>
+      <c r="C14" s="233" t="s">
         <v>400</v>
       </c>
-      <c r="D14" s="234" t="s">
+      <c r="D14" s="229" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="235" t="s">
+      <c r="E14" s="230" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="235" t="s">
+      <c r="F14" s="230" t="s">
         <v>215</v>
       </c>
-      <c r="G14" s="240" t="s">
+      <c r="G14" s="235" t="s">
         <v>403</v>
       </c>
-      <c r="H14" s="239"/>
-      <c r="I14" s="239"/>
+      <c r="H14" s="234"/>
+      <c r="I14" s="234"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="273"/>
-      <c r="C15" s="242" t="s">
+      <c r="B15" s="268"/>
+      <c r="C15" s="237" t="s">
         <v>401</v>
       </c>
-      <c r="D15" s="236" t="s">
+      <c r="D15" s="231" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="237" t="s">
+      <c r="E15" s="232" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="237" t="s">
+      <c r="F15" s="232" t="s">
         <v>215</v>
       </c>
-      <c r="G15" s="242" t="s">
+      <c r="G15" s="237" t="s">
         <v>405</v>
       </c>
-      <c r="H15" s="243"/>
-      <c r="I15" s="238" t="s">
+      <c r="H15" s="238"/>
+      <c r="I15" s="233" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="264" t="s">
+      <c r="B16" s="259" t="s">
         <v>38</v>
       </c>
       <c r="C16" s="72" t="s">
@@ -5641,13 +5640,13 @@
       <c r="G16" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="H16" s="270"/>
+      <c r="H16" s="265"/>
       <c r="I16" s="7" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="17" spans="2:33" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="265"/>
+      <c r="B17" s="260"/>
       <c r="C17" s="66" t="s">
         <v>237</v>
       </c>
@@ -5663,11 +5662,11 @@
       <c r="G17" s="67" t="s">
         <v>208</v>
       </c>
-      <c r="H17" s="270"/>
+      <c r="H17" s="265"/>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="2:33" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="265"/>
+      <c r="B18" s="260"/>
       <c r="C18" s="66" t="s">
         <v>42</v>
       </c>
@@ -5683,13 +5682,13 @@
       <c r="G18" s="67" t="s">
         <v>242</v>
       </c>
-      <c r="H18" s="270"/>
-      <c r="I18" s="262" t="s">
+      <c r="H18" s="265"/>
+      <c r="I18" s="257" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="19" spans="2:33" ht="146.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="266"/>
+      <c r="B19" s="261"/>
       <c r="C19" s="80" t="s">
         <v>43</v>
       </c>
@@ -5705,11 +5704,11 @@
       <c r="G19" s="81" t="s">
         <v>209</v>
       </c>
-      <c r="H19" s="271"/>
-      <c r="I19" s="263"/>
+      <c r="H19" s="266"/>
+      <c r="I19" s="258"/>
     </row>
     <row r="20" spans="2:33" ht="80.099999999999994" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="280" t="s">
+      <c r="B20" s="275" t="s">
         <v>203</v>
       </c>
       <c r="C20" s="72" t="s">
@@ -5727,13 +5726,13 @@
       <c r="G20" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="277" t="s">
+      <c r="H20" s="272" t="s">
         <v>236</v>
       </c>
       <c r="I20" s="23"/>
     </row>
     <row r="21" spans="2:33" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="268"/>
+      <c r="B21" s="263"/>
       <c r="C21" s="66" t="s">
         <v>46</v>
       </c>
@@ -5749,11 +5748,11 @@
       <c r="G21" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="H21" s="278"/>
+      <c r="H21" s="273"/>
       <c r="I21" s="22"/>
     </row>
     <row r="22" spans="2:33" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="268"/>
+      <c r="B22" s="263"/>
       <c r="C22" s="67" t="s">
         <v>48</v>
       </c>
@@ -5769,11 +5768,11 @@
       <c r="G22" s="67" t="s">
         <v>204</v>
       </c>
-      <c r="H22" s="278"/>
+      <c r="H22" s="273"/>
       <c r="I22" s="22"/>
     </row>
     <row r="23" spans="2:33" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B23" s="268"/>
+      <c r="B23" s="263"/>
       <c r="C23" s="68" t="s">
         <v>206</v>
       </c>
@@ -5789,11 +5788,11 @@
       <c r="G23" s="69" t="s">
         <v>245</v>
       </c>
-      <c r="H23" s="278"/>
+      <c r="H23" s="273"/>
       <c r="I23" s="22"/>
     </row>
     <row r="24" spans="2:33" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="268"/>
+      <c r="B24" s="263"/>
       <c r="C24" s="74" t="s">
         <v>207</v>
       </c>
@@ -5809,11 +5808,11 @@
       <c r="G24" s="76" t="s">
         <v>292</v>
       </c>
-      <c r="H24" s="279"/>
+      <c r="H24" s="274"/>
       <c r="I24" s="22"/>
     </row>
     <row r="25" spans="2:33" ht="26.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="267" t="s">
+      <c r="B25" s="262" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="77" t="s">
@@ -5837,7 +5836,7 @@
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="2:33" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="268"/>
+      <c r="B26" s="263"/>
       <c r="C26" s="67" t="s">
         <v>53</v>
       </c>
@@ -5853,11 +5852,11 @@
       <c r="G26" s="69" t="s">
         <v>246</v>
       </c>
-      <c r="H26" s="281"/>
+      <c r="H26" s="276"/>
       <c r="I26" s="65"/>
     </row>
     <row r="27" spans="2:33" ht="115.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="269"/>
+      <c r="B27" s="264"/>
       <c r="C27" s="72" t="s">
         <v>51</v>
       </c>
@@ -5867,17 +5866,17 @@
       <c r="E27" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="168" t="s">
+      <c r="F27" s="166" t="s">
         <v>235</v>
       </c>
       <c r="G27" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="H27" s="282"/>
+      <c r="H27" s="277"/>
       <c r="I27" s="65"/>
     </row>
     <row r="28" spans="2:33" ht="51.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="267" t="s">
+      <c r="B28" s="262" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="77" t="s">
@@ -5908,7 +5907,7 @@
       <c r="AG28" s="4"/>
     </row>
     <row r="29" spans="2:33" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B29" s="268"/>
+      <c r="B29" s="263"/>
       <c r="C29" s="72" t="s">
         <v>249</v>
       </c>
@@ -5937,7 +5936,7 @@
       <c r="AG29" s="4"/>
     </row>
     <row r="30" spans="2:33" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="268"/>
+      <c r="B30" s="263"/>
       <c r="C30" s="72" t="s">
         <v>255</v>
       </c>
@@ -5953,7 +5952,7 @@
       <c r="G30" s="67" t="s">
         <v>253</v>
       </c>
-      <c r="H30" s="281"/>
+      <c r="H30" s="276"/>
       <c r="I30" s="3"/>
       <c r="Y30" s="6"/>
       <c r="Z30" s="6"/>
@@ -5966,7 +5965,7 @@
       <c r="AG30" s="4"/>
     </row>
     <row r="31" spans="2:33" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="268"/>
+      <c r="B31" s="263"/>
       <c r="C31" s="72" t="s">
         <v>256</v>
       </c>
@@ -5982,7 +5981,7 @@
       <c r="G31" s="94" t="s">
         <v>254</v>
       </c>
-      <c r="H31" s="283"/>
+      <c r="H31" s="278"/>
       <c r="I31" s="3"/>
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
@@ -5995,7 +5994,7 @@
       <c r="AG31" s="4"/>
     </row>
     <row r="32" spans="2:33" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="268"/>
+      <c r="B32" s="263"/>
       <c r="C32" s="67" t="s">
         <v>57</v>
       </c>
@@ -6011,7 +6010,7 @@
       <c r="G32" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="H32" s="283"/>
+      <c r="H32" s="278"/>
       <c r="I32" s="3"/>
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
@@ -6024,7 +6023,7 @@
       <c r="AG32" s="4"/>
     </row>
     <row r="33" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="268"/>
+      <c r="B33" s="263"/>
       <c r="C33" s="67" t="s">
         <v>56</v>
       </c>
@@ -6040,11 +6039,11 @@
       <c r="G33" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="H33" s="284"/>
+      <c r="H33" s="279"/>
       <c r="I33" s="11"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="268"/>
+      <c r="B34" s="263"/>
       <c r="C34" s="67" t="s">
         <v>59</v>
       </c>
@@ -6064,7 +6063,7 @@
       <c r="I34" s="11"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="268"/>
+      <c r="B35" s="263"/>
       <c r="C35" s="95" t="s">
         <v>61</v>
       </c>
@@ -6082,7 +6081,7 @@
       <c r="I35" s="11"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="268"/>
+      <c r="B36" s="263"/>
       <c r="C36" s="95" t="s">
         <v>63</v>
       </c>
@@ -6100,7 +6099,7 @@
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="268"/>
+      <c r="B37" s="263"/>
       <c r="C37" s="95" t="s">
         <v>65</v>
       </c>
@@ -6118,7 +6117,7 @@
       <c r="I37" s="11"/>
     </row>
     <row r="38" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="269"/>
+      <c r="B38" s="264"/>
       <c r="C38" s="96" t="s">
         <v>67</v>
       </c>
@@ -6136,7 +6135,7 @@
       <c r="I38" s="11"/>
     </row>
     <row r="39" spans="2:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="267" t="s">
+      <c r="B39" s="262" t="s">
         <v>69</v>
       </c>
       <c r="C39" s="85" t="s">
@@ -6156,7 +6155,7 @@
       <c r="I39" s="11"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="268"/>
+      <c r="B40" s="263"/>
       <c r="C40" s="70" t="s">
         <v>72</v>
       </c>
@@ -6174,7 +6173,7 @@
       <c r="I40" s="11"/>
     </row>
     <row r="41" spans="2:9" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B41" s="268"/>
+      <c r="B41" s="263"/>
       <c r="C41" s="70" t="s">
         <v>74</v>
       </c>
@@ -6192,7 +6191,7 @@
       <c r="I41" s="11"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="268"/>
+      <c r="B42" s="263"/>
       <c r="C42" s="70" t="s">
         <v>76</v>
       </c>
@@ -6209,20 +6208,20 @@
       <c r="H42" s="83"/>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="2:9" s="180" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="269"/>
-      <c r="C43" s="178" t="s">
+    <row r="43" spans="2:9" s="178" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="264"/>
+      <c r="C43" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="178"/>
-      <c r="E43" s="178"/>
-      <c r="F43" s="178"/>
-      <c r="G43" s="178"/>
-      <c r="H43" s="178"/>
-      <c r="I43" s="179"/>
+      <c r="D43" s="176"/>
+      <c r="E43" s="176"/>
+      <c r="F43" s="176"/>
+      <c r="G43" s="176"/>
+      <c r="H43" s="176"/>
+      <c r="I43" s="177"/>
     </row>
     <row r="44" spans="2:9" ht="51.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="267" t="s">
+      <c r="B44" s="262" t="s">
         <v>80</v>
       </c>
       <c r="C44" s="85" t="s">
@@ -6238,12 +6237,12 @@
       <c r="G44" s="89" t="s">
         <v>238</v>
       </c>
-      <c r="I44" s="158" t="s">
+      <c r="I44" s="157" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B45" s="268"/>
+      <c r="B45" s="263"/>
       <c r="C45" s="70" t="s">
         <v>82</v>
       </c>
@@ -6261,7 +6260,7 @@
       <c r="I45" s="11"/>
     </row>
     <row r="46" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B46" s="268"/>
+      <c r="B46" s="263"/>
       <c r="C46" s="70" t="s">
         <v>83</v>
       </c>
@@ -6279,7 +6278,7 @@
       <c r="I46" s="11"/>
     </row>
     <row r="47" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B47" s="268"/>
+      <c r="B47" s="263"/>
       <c r="C47" s="70" t="s">
         <v>84</v>
       </c>
@@ -6297,7 +6296,7 @@
       <c r="I47" s="11"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="268"/>
+      <c r="B48" s="263"/>
       <c r="C48" s="70" t="s">
         <v>86</v>
       </c>
@@ -6314,20 +6313,20 @@
       <c r="H48" s="83"/>
       <c r="I48" s="11"/>
     </row>
-    <row r="49" spans="2:9" s="180" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="269"/>
-      <c r="C49" s="178" t="s">
+    <row r="49" spans="2:9" s="178" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="264"/>
+      <c r="C49" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="D49" s="178"/>
-      <c r="E49" s="178"/>
-      <c r="F49" s="178"/>
-      <c r="G49" s="178"/>
-      <c r="H49" s="178"/>
-      <c r="I49" s="179"/>
+      <c r="D49" s="176"/>
+      <c r="E49" s="176"/>
+      <c r="F49" s="176"/>
+      <c r="G49" s="176"/>
+      <c r="H49" s="176"/>
+      <c r="I49" s="177"/>
     </row>
     <row r="50" spans="2:9" ht="26.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="267" t="s">
+      <c r="B50" s="262" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="87" t="s">
@@ -6347,7 +6346,7 @@
       <c r="I50" s="11"/>
     </row>
     <row r="51" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B51" s="268"/>
+      <c r="B51" s="263"/>
       <c r="C51" s="71" t="s">
         <v>91</v>
       </c>
@@ -6364,79 +6363,79 @@
       <c r="H51" s="83"/>
       <c r="I51" s="11"/>
     </row>
-    <row r="52" spans="2:9" s="180" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="269"/>
-      <c r="C52" s="178" t="s">
+    <row r="52" spans="2:9" s="178" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="264"/>
+      <c r="C52" s="176" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="178"/>
-      <c r="E52" s="178"/>
-      <c r="F52" s="178"/>
-      <c r="G52" s="178"/>
-      <c r="H52" s="178"/>
-      <c r="I52" s="179"/>
+      <c r="D52" s="176"/>
+      <c r="E52" s="176"/>
+      <c r="F52" s="176"/>
+      <c r="G52" s="176"/>
+      <c r="H52" s="176"/>
+      <c r="I52" s="177"/>
     </row>
     <row r="53" spans="2:9" ht="39.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="181" t="s">
+      <c r="B53" s="179" t="s">
         <v>259</v>
       </c>
-      <c r="C53" s="182" t="s">
+      <c r="C53" s="180" t="s">
         <v>260</v>
       </c>
-      <c r="D53" s="183" t="s">
+      <c r="D53" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="E53" s="201" t="s">
+      <c r="E53" s="197" t="s">
         <v>29</v>
       </c>
-      <c r="F53" s="184" t="s">
+      <c r="F53" s="182" t="s">
         <v>215</v>
       </c>
-      <c r="G53" s="183" t="s">
+      <c r="G53" s="181" t="s">
         <v>261</v>
       </c>
-      <c r="H53" s="150"/>
-      <c r="I53" s="151"/>
+      <c r="H53" s="149"/>
+      <c r="I53" s="150"/>
     </row>
     <row r="54" spans="2:9" ht="51.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="285" t="s">
+      <c r="B54" s="280" t="s">
         <v>93</v>
       </c>
-      <c r="C54" s="185" t="s">
+      <c r="C54" s="183" t="s">
         <v>262</v>
       </c>
-      <c r="D54" s="186" t="s">
+      <c r="D54" s="184" t="s">
         <v>40</v>
       </c>
-      <c r="E54" s="202" t="s">
+      <c r="E54" s="198" t="s">
         <v>287</v>
       </c>
-      <c r="F54" s="187" t="s">
+      <c r="F54" s="185" t="s">
         <v>215</v>
       </c>
-      <c r="G54" s="185" t="s">
+      <c r="G54" s="183" t="s">
         <v>263</v>
       </c>
-      <c r="H54" s="152"/>
+      <c r="H54" s="151"/>
       <c r="I54" s="5" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="55" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B55" s="286"/>
-      <c r="C55" s="188" t="s">
+      <c r="B55" s="281"/>
+      <c r="C55" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="D55" s="188" t="s">
+      <c r="D55" s="186" t="s">
         <v>40</v>
       </c>
-      <c r="E55" s="188" t="s">
+      <c r="E55" s="186" t="s">
         <v>26</v>
       </c>
-      <c r="F55" s="189" t="s">
+      <c r="F55" s="187" t="s">
         <v>215</v>
       </c>
-      <c r="G55" s="188" t="s">
+      <c r="G55" s="186" t="s">
         <v>264</v>
       </c>
       <c r="H55" s="5" t="s">
@@ -6444,30 +6443,30 @@
       </c>
     </row>
     <row r="56" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B56" s="286"/>
-      <c r="C56" s="190" t="s">
+      <c r="B56" s="281"/>
+      <c r="C56" s="188" t="s">
         <v>102</v>
       </c>
-      <c r="D56" s="190" t="s">
+      <c r="D56" s="188" t="s">
         <v>23</v>
       </c>
-      <c r="E56" s="190" t="s">
+      <c r="E56" s="188" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="191" t="s">
+      <c r="F56" s="189" t="s">
         <v>215</v>
       </c>
-      <c r="G56" s="190" t="s">
+      <c r="G56" s="188" t="s">
         <v>276</v>
       </c>
       <c r="H56" s="132"/>
     </row>
     <row r="57" spans="2:9" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="286"/>
-      <c r="C57" s="188" t="s">
+      <c r="B57" s="281"/>
+      <c r="C57" s="186" t="s">
         <v>277</v>
       </c>
-      <c r="D57" s="192" t="s">
+      <c r="D57" s="190" t="s">
         <v>23</v>
       </c>
       <c r="E57" s="10" t="s">
@@ -6479,14 +6478,14 @@
       <c r="G57" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="H57" s="193"/>
+      <c r="H57" s="191"/>
     </row>
     <row r="58" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B58" s="286"/>
+      <c r="B58" s="281"/>
       <c r="C58" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="D58" s="192" t="s">
+      <c r="D58" s="190" t="s">
         <v>40</v>
       </c>
       <c r="E58" s="10" t="s">
@@ -6500,18 +6499,18 @@
       </c>
       <c r="H58" s="132"/>
     </row>
-    <row r="59" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B59" s="286"/>
-      <c r="C59" s="194" t="s">
+    <row r="59" spans="2:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="281"/>
+      <c r="C59" s="192" t="s">
         <v>279</v>
       </c>
-      <c r="D59" s="194" t="s">
+      <c r="D59" s="192" t="s">
         <v>40</v>
       </c>
       <c r="E59" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="F59" s="195" t="s">
+      <c r="F59" s="193" t="s">
         <v>235</v>
       </c>
       <c r="G59" s="31" t="s">
@@ -6519,144 +6518,144 @@
       </c>
       <c r="H59" s="132"/>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B60" s="286"/>
-      <c r="C60" s="153" t="s">
+    <row r="60" spans="2:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="281"/>
+      <c r="C60" s="89" t="s">
         <v>94</v>
       </c>
-      <c r="D60" s="153" t="s">
+      <c r="D60" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E60" s="203" t="s">
+      <c r="E60" s="289" t="s">
         <v>41</v>
       </c>
-      <c r="F60" s="167" t="s">
+      <c r="F60" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="G60" s="153" t="s">
+      <c r="G60" s="89" t="s">
         <v>265</v>
       </c>
       <c r="H60" s="132"/>
     </row>
-    <row r="61" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B61" s="286"/>
-      <c r="C61" s="188" t="s">
+    <row r="61" spans="2:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="281"/>
+      <c r="C61" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="188" t="s">
+      <c r="D61" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E61" s="188" t="s">
+      <c r="E61" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="F61" s="189" t="s">
+      <c r="F61" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="G61" s="188" t="s">
+      <c r="G61" s="89" t="s">
         <v>266</v>
       </c>
       <c r="H61" s="132"/>
     </row>
-    <row r="62" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B62" s="286"/>
-      <c r="C62" s="188" t="s">
+    <row r="62" spans="2:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="281"/>
+      <c r="C62" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="D62" s="188" t="s">
+      <c r="D62" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E62" s="188" t="s">
+      <c r="E62" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="F62" s="189" t="s">
+      <c r="F62" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="G62" s="188" t="s">
+      <c r="G62" s="89" t="s">
         <v>267</v>
       </c>
       <c r="H62" s="132"/>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B63" s="286"/>
-      <c r="C63" s="188" t="s">
+    <row r="63" spans="2:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="281"/>
+      <c r="C63" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="D63" s="188" t="s">
+      <c r="D63" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E63" s="188" t="s">
+      <c r="E63" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="F63" s="189" t="s">
+      <c r="F63" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="G63" s="188" t="s">
+      <c r="G63" s="89" t="s">
         <v>268</v>
       </c>
       <c r="H63" s="132"/>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B64" s="286"/>
-      <c r="C64" s="188" t="s">
+    <row r="64" spans="2:9" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="281"/>
+      <c r="C64" s="89" t="s">
         <v>99</v>
       </c>
-      <c r="D64" s="188" t="s">
+      <c r="D64" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E64" s="188" t="s">
+      <c r="E64" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="F64" s="189" t="s">
+      <c r="F64" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="G64" s="188" t="s">
+      <c r="G64" s="89" t="s">
         <v>269</v>
       </c>
       <c r="H64" s="132"/>
     </row>
-    <row r="65" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B65" s="286"/>
-      <c r="C65" s="188" t="s">
+    <row r="65" spans="2:10" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="281"/>
+      <c r="C65" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="D65" s="188" t="s">
+      <c r="D65" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E65" s="188" t="s">
+      <c r="E65" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="F65" s="189" t="s">
+      <c r="F65" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="G65" s="188" t="s">
+      <c r="G65" s="89" t="s">
         <v>270</v>
       </c>
       <c r="H65" s="132"/>
     </row>
-    <row r="66" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="287"/>
-      <c r="C66" s="196" t="s">
+    <row r="66" spans="2:10" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="282"/>
+      <c r="C66" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="D66" s="196" t="s">
+      <c r="D66" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E66" s="196" t="s">
+      <c r="E66" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="F66" s="197" t="s">
+      <c r="F66" s="89" t="s">
         <v>215</v>
       </c>
-      <c r="G66" s="196" t="s">
+      <c r="G66" s="89" t="s">
         <v>271</v>
       </c>
-      <c r="H66" s="148"/>
+      <c r="H66" s="147"/>
     </row>
     <row r="67" spans="2:10" ht="51.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="274" t="s">
+      <c r="B67" s="269" t="s">
         <v>103</v>
       </c>
-      <c r="C67" s="159" t="s">
+      <c r="C67" s="158" t="s">
         <v>103</v>
       </c>
       <c r="D67" s="88" t="s">
@@ -6665,22 +6664,22 @@
       <c r="E67" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="F67" s="160"/>
+      <c r="F67" s="159"/>
       <c r="G67" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="H67" s="154" t="s">
+      <c r="H67" s="153" t="s">
         <v>272</v>
       </c>
-      <c r="I67" s="155" t="s">
+      <c r="I67" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="J67" s="155" t="s">
+      <c r="J67" s="154" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="68" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="275"/>
+      <c r="B68" s="270"/>
       <c r="C68" s="92" t="s">
         <v>275</v>
       </c>
@@ -6690,15 +6689,15 @@
       <c r="E68" s="92" t="s">
         <v>26</v>
       </c>
-      <c r="F68" s="161"/>
+      <c r="F68" s="160"/>
       <c r="G68" s="93" t="s">
         <v>244</v>
       </c>
-      <c r="H68" s="156"/>
-      <c r="I68" s="157"/>
+      <c r="H68" s="155"/>
+      <c r="I68" s="156"/>
     </row>
     <row r="69" spans="2:10" ht="26.25" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="274" t="s">
+      <c r="B69" s="269" t="s">
         <v>106</v>
       </c>
       <c r="C69" s="88" t="s">
@@ -6710,14 +6709,14 @@
       <c r="E69" s="88" t="s">
         <v>41</v>
       </c>
-      <c r="F69" s="160"/>
+      <c r="F69" s="159"/>
       <c r="G69" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="H69" s="152"/>
+      <c r="H69" s="151"/>
     </row>
     <row r="70" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B70" s="276"/>
+      <c r="B70" s="271"/>
       <c r="C70" s="90" t="s">
         <v>107</v>
       </c>
@@ -6727,14 +6726,14 @@
       <c r="E70" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="F70" s="162"/>
+      <c r="F70" s="161"/>
       <c r="G70" s="91" t="s">
         <v>108</v>
       </c>
       <c r="H70" s="132"/>
     </row>
     <row r="71" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B71" s="276"/>
+      <c r="B71" s="271"/>
       <c r="C71" s="90" t="s">
         <v>109</v>
       </c>
@@ -6744,14 +6743,14 @@
       <c r="E71" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="F71" s="162"/>
+      <c r="F71" s="161"/>
       <c r="G71" s="91" t="s">
         <v>110</v>
       </c>
       <c r="H71" s="132"/>
     </row>
     <row r="72" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="275"/>
+      <c r="B72" s="270"/>
       <c r="C72" s="92" t="s">
         <v>111</v>
       </c>
@@ -6761,21 +6760,21 @@
       <c r="E72" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="F72" s="161"/>
+      <c r="F72" s="160"/>
       <c r="G72" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="H72" s="148"/>
+      <c r="H72" s="147"/>
     </row>
     <row r="73" spans="2:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="163"/>
-      <c r="C73" s="164" t="s">
+      <c r="B73" s="162"/>
+      <c r="C73" s="163" t="s">
         <v>113</v>
       </c>
-      <c r="D73" s="165"/>
-      <c r="E73" s="165"/>
-      <c r="F73" s="166"/>
-      <c r="G73" s="166"/>
+      <c r="D73" s="164"/>
+      <c r="E73" s="164"/>
+      <c r="F73" s="165"/>
+      <c r="G73" s="165"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -6809,7 +6808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="75" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -6860,10 +6859,10 @@
       <c r="H6" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="252" t="s">
+      <c r="A8" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="247"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -6880,10 +6879,10 @@
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="254" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="259"/>
+      <c r="B10" s="254"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -6923,7 +6922,7 @@
       <c r="M12" s="53"/>
     </row>
     <row r="13" spans="1:13" ht="90" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="260" t="s">
+      <c r="A13" s="255" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -6951,12 +6950,12 @@
       <c r="J13" s="45" t="s">
         <v>161</v>
       </c>
-      <c r="K13" s="207"/>
+      <c r="K13" s="202"/>
       <c r="L13" s="45"/>
       <c r="M13" s="120"/>
     </row>
     <row r="14" spans="1:13" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="250"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="10" t="s">
         <v>7</v>
       </c>
@@ -6979,7 +6978,7 @@
       <c r="M14" s="121"/>
     </row>
     <row r="15" spans="1:13" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="253" t="s">
+      <c r="A15" s="248" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -7006,7 +7005,7 @@
       <c r="M15" s="120"/>
     </row>
     <row r="16" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="257"/>
+      <c r="A16" s="252"/>
       <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
@@ -7031,27 +7030,27 @@
       <c r="M16" s="124"/>
     </row>
     <row r="17" spans="1:33" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="254"/>
+      <c r="A17" s="249"/>
       <c r="B17" s="36" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="55"/>
-      <c r="E17" s="225" t="s">
+      <c r="E17" s="220" t="s">
         <v>293</v>
       </c>
-      <c r="F17" s="226" t="s">
+      <c r="F17" s="221" t="s">
         <v>294</v>
       </c>
-      <c r="G17" s="205"/>
-      <c r="H17" s="147"/>
-      <c r="I17" s="148"/>
+      <c r="G17" s="200"/>
+      <c r="H17" s="146"/>
+      <c r="I17" s="147"/>
       <c r="J17" s="46"/>
       <c r="K17" s="46"/>
       <c r="L17" s="46"/>
       <c r="M17" s="121"/>
     </row>
     <row r="18" spans="1:33" ht="64.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="256" t="s">
+      <c r="A18" s="251" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="38" t="s">
@@ -7078,7 +7077,7 @@
       <c r="M18" s="122"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="254"/>
+      <c r="A19" s="249"/>
       <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
@@ -7095,7 +7094,7 @@
       <c r="M19" s="121"/>
     </row>
     <row r="20" spans="1:33" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="255"/>
+      <c r="A20" s="250"/>
       <c r="B20" s="36" t="s">
         <v>16</v>
       </c>
@@ -7112,7 +7111,7 @@
       <c r="M20" s="123"/>
     </row>
     <row r="21" spans="1:33" ht="159.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="290" t="s">
+      <c r="A21" s="285" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="30" t="s">
@@ -7129,13 +7128,13 @@
       <c r="G21" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="H21" s="210" t="s">
+      <c r="H21" s="205" t="s">
         <v>130</v>
       </c>
       <c r="I21" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="J21" s="204" t="s">
+      <c r="J21" s="199" t="s">
         <v>295</v>
       </c>
       <c r="K21" s="49" t="s">
@@ -7145,7 +7144,7 @@
       <c r="M21" s="124"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A22" s="291"/>
+      <c r="A22" s="286"/>
       <c r="B22" s="10" t="s">
         <v>172</v>
       </c>
@@ -7156,13 +7155,13 @@
       <c r="E22" s="99" t="s">
         <v>224</v>
       </c>
-      <c r="F22" s="229" t="s">
+      <c r="F22" s="224" t="s">
         <v>391</v>
       </c>
-      <c r="G22" s="229" t="s">
+      <c r="G22" s="224" t="s">
         <v>392</v>
       </c>
-      <c r="H22" s="229" t="s">
+      <c r="H22" s="224" t="s">
         <v>393</v>
       </c>
       <c r="I22" s="46"/>
@@ -7172,7 +7171,7 @@
       <c r="M22" s="121"/>
     </row>
     <row r="23" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="291"/>
+      <c r="A23" s="286"/>
       <c r="B23" s="10" t="s">
         <v>196</v>
       </c>
@@ -7189,13 +7188,13 @@
       <c r="G23" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="H23" s="229" t="s">
+      <c r="H23" s="224" t="s">
         <v>394</v>
       </c>
-      <c r="I23" s="229" t="s">
+      <c r="I23" s="224" t="s">
         <v>411</v>
       </c>
-      <c r="J23" s="229" t="s">
+      <c r="J23" s="224" t="s">
         <v>413</v>
       </c>
       <c r="K23" s="46"/>
@@ -7203,7 +7202,7 @@
       <c r="M23" s="121"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A24" s="291"/>
+      <c r="A24" s="286"/>
       <c r="B24" s="10" t="s">
         <v>197</v>
       </c>
@@ -7222,7 +7221,7 @@
       <c r="M24" s="121"/>
     </row>
     <row r="25" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="291"/>
+      <c r="A25" s="286"/>
       <c r="B25" s="63" t="s">
         <v>170</v>
       </c>
@@ -7245,7 +7244,7 @@
       <c r="M25" s="125"/>
     </row>
     <row r="26" spans="1:33" ht="258" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="292"/>
+      <c r="A26" s="287"/>
       <c r="B26" s="36" t="s">
         <v>18</v>
       </c>
@@ -7265,7 +7264,7 @@
       <c r="H26" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="I26" s="248" t="s">
+      <c r="I26" s="243" t="s">
         <v>122</v>
       </c>
       <c r="J26" s="48"/>
@@ -7283,7 +7282,7 @@
       <c r="AG26" s="4"/>
     </row>
     <row r="27" spans="1:33" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="267" t="s">
+      <c r="A27" s="262" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="42" t="s">
@@ -7297,13 +7296,13 @@
       <c r="F27" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="G27" s="228" t="s">
+      <c r="G27" s="223" t="s">
         <v>396</v>
       </c>
-      <c r="H27" s="228" t="s">
+      <c r="H27" s="223" t="s">
         <v>397</v>
       </c>
-      <c r="I27" s="228" t="s">
+      <c r="I27" s="223" t="s">
         <v>398</v>
       </c>
       <c r="J27" s="102"/>
@@ -7312,25 +7311,25 @@
       <c r="M27" s="126"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A28" s="268"/>
-      <c r="B28" s="240" t="s">
+      <c r="A28" s="263"/>
+      <c r="B28" s="235" t="s">
         <v>399</v>
       </c>
-      <c r="C28" s="238"/>
+      <c r="C28" s="233"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="238" t="s">
+      <c r="E28" s="233" t="s">
         <v>175</v>
       </c>
-      <c r="F28" s="238" t="s">
+      <c r="F28" s="233" t="s">
         <v>174</v>
       </c>
-      <c r="G28" s="238" t="s">
+      <c r="G28" s="233" t="s">
         <v>396</v>
       </c>
-      <c r="H28" s="238" t="s">
+      <c r="H28" s="233" t="s">
         <v>397</v>
       </c>
-      <c r="I28" s="238" t="s">
+      <c r="I28" s="233" t="s">
         <v>398</v>
       </c>
       <c r="J28" s="10"/>
@@ -7339,25 +7338,25 @@
       <c r="M28" s="10"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A29" s="268"/>
-      <c r="B29" s="240" t="s">
+      <c r="A29" s="263"/>
+      <c r="B29" s="235" t="s">
         <v>400</v>
       </c>
-      <c r="C29" s="238"/>
+      <c r="C29" s="233"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="238" t="s">
+      <c r="E29" s="233" t="s">
         <v>175</v>
       </c>
-      <c r="F29" s="238" t="s">
+      <c r="F29" s="233" t="s">
         <v>174</v>
       </c>
-      <c r="G29" s="238" t="s">
+      <c r="G29" s="233" t="s">
         <v>396</v>
       </c>
-      <c r="H29" s="238" t="s">
+      <c r="H29" s="233" t="s">
         <v>397</v>
       </c>
-      <c r="I29" s="238" t="s">
+      <c r="I29" s="233" t="s">
         <v>398</v>
       </c>
       <c r="J29" s="10"/>
@@ -7366,18 +7365,18 @@
       <c r="M29" s="10"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A30" s="293"/>
-      <c r="B30" s="240" t="s">
+      <c r="A30" s="288"/>
+      <c r="B30" s="235" t="s">
         <v>401</v>
       </c>
-      <c r="C30" s="238"/>
+      <c r="C30" s="233"/>
       <c r="D30" s="55"/>
-      <c r="E30" s="244" t="s">
+      <c r="E30" s="239" t="s">
         <v>412</v>
       </c>
-      <c r="F30" s="244"/>
+      <c r="F30" s="239"/>
       <c r="G30" s="132"/>
-      <c r="H30" s="172"/>
+      <c r="H30" s="170"/>
       <c r="I30" s="132"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -7400,7 +7399,7 @@
       <c r="M31" s="127"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A32" s="257" t="s">
+      <c r="A32" s="252" t="s">
         <v>203</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -7445,7 +7444,7 @@
       <c r="W32" s="9"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="254"/>
+      <c r="A33" s="249"/>
       <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
@@ -7502,22 +7501,22 @@
       <c r="W33" s="9"/>
     </row>
     <row r="34" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="258"/>
+      <c r="A34" s="253"/>
       <c r="B34" s="41" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="50"/>
       <c r="D34" s="55"/>
-      <c r="E34" s="225" t="s">
+      <c r="E34" s="220" t="s">
         <v>304</v>
       </c>
-      <c r="F34" s="225" t="s">
+      <c r="F34" s="220" t="s">
         <v>305</v>
       </c>
-      <c r="G34" s="225" t="s">
+      <c r="G34" s="220" t="s">
         <v>306</v>
       </c>
-      <c r="H34" s="225" t="s">
+      <c r="H34" s="220" t="s">
         <v>151</v>
       </c>
       <c r="I34" s="129"/>
@@ -7614,7 +7613,7 @@
         <v>249</v>
       </c>
       <c r="C37" s="48"/>
-      <c r="D37" s="176"/>
+      <c r="D37" s="174"/>
       <c r="E37" s="131" t="s">
         <v>252</v>
       </c>
@@ -7640,14 +7639,14 @@
       <c r="W37" s="9"/>
     </row>
     <row r="38" spans="1:23" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="288" t="s">
+      <c r="A38" s="283" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="198" t="s">
+      <c r="B38" s="194" t="s">
         <v>262</v>
       </c>
       <c r="C38" s="30"/>
-      <c r="D38" s="174"/>
+      <c r="D38" s="172"/>
       <c r="E38" s="30" t="s">
         <v>281</v>
       </c>
@@ -7657,18 +7656,18 @@
       <c r="G38" s="30"/>
       <c r="H38" s="30"/>
       <c r="I38" s="30"/>
-      <c r="J38" s="173"/>
-      <c r="K38" s="175"/>
-      <c r="L38" s="175"/>
-      <c r="M38" s="175"/>
+      <c r="J38" s="171"/>
+      <c r="K38" s="173"/>
+      <c r="L38" s="173"/>
+      <c r="M38" s="173"/>
     </row>
     <row r="39" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A39" s="289"/>
-      <c r="B39" s="188" t="s">
+      <c r="A39" s="284"/>
+      <c r="B39" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="C39" s="193"/>
-      <c r="D39" s="199"/>
+      <c r="C39" s="191"/>
+      <c r="D39" s="195"/>
       <c r="E39" s="10" t="s">
         <v>115</v>
       </c>
@@ -7684,37 +7683,37 @@
       <c r="I39" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="J39" s="169"/>
+      <c r="J39" s="167"/>
       <c r="K39" s="132"/>
       <c r="L39" s="132"/>
       <c r="M39" s="132"/>
     </row>
     <row r="40" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="289"/>
-      <c r="B40" s="188" t="s">
+      <c r="A40" s="284"/>
+      <c r="B40" s="186" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="193"/>
-      <c r="D40" s="199"/>
-      <c r="E40" s="222" t="s">
+      <c r="C40" s="191"/>
+      <c r="D40" s="195"/>
+      <c r="E40" s="217" t="s">
         <v>284</v>
       </c>
-      <c r="F40" s="193"/>
-      <c r="G40" s="193"/>
-      <c r="H40" s="200"/>
-      <c r="I40" s="193"/>
+      <c r="F40" s="191"/>
+      <c r="G40" s="191"/>
+      <c r="H40" s="196"/>
+      <c r="I40" s="191"/>
       <c r="J40" s="132"/>
       <c r="K40" s="132"/>
       <c r="L40" s="132"/>
       <c r="M40" s="132"/>
     </row>
     <row r="41" spans="1:23" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A41" s="289"/>
-      <c r="B41" s="188" t="s">
+      <c r="A41" s="284"/>
+      <c r="B41" s="186" t="s">
         <v>277</v>
       </c>
-      <c r="C41" s="193"/>
-      <c r="D41" s="199"/>
+      <c r="C41" s="191"/>
+      <c r="D41" s="195"/>
       <c r="E41" s="10" t="s">
         <v>153</v>
       </c>
@@ -7734,18 +7733,18 @@
       <c r="M41" s="132"/>
     </row>
     <row r="42" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="289"/>
-      <c r="B42" s="153" t="s">
+      <c r="A42" s="284"/>
+      <c r="B42" s="152" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="170" t="s">
+      <c r="C42" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D42" s="171"/>
+      <c r="D42" s="169"/>
       <c r="E42" s="132"/>
       <c r="F42" s="132"/>
       <c r="G42" s="132"/>
-      <c r="H42" s="172"/>
+      <c r="H42" s="170"/>
       <c r="I42" s="132"/>
       <c r="J42" s="132"/>
       <c r="K42" s="132"/>
@@ -7753,18 +7752,18 @@
       <c r="M42" s="132"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A43" s="289"/>
-      <c r="B43" s="153" t="s">
+      <c r="A43" s="284"/>
+      <c r="B43" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="170" t="s">
+      <c r="C43" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D43" s="171"/>
+      <c r="D43" s="169"/>
       <c r="E43" s="132"/>
       <c r="F43" s="132"/>
       <c r="G43" s="132"/>
-      <c r="H43" s="172"/>
+      <c r="H43" s="170"/>
       <c r="I43" s="132"/>
       <c r="J43" s="132"/>
       <c r="K43" s="132"/>
@@ -7772,18 +7771,18 @@
       <c r="M43" s="132"/>
     </row>
     <row r="44" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="289"/>
-      <c r="B44" s="153" t="s">
+      <c r="A44" s="284"/>
+      <c r="B44" s="152" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="170" t="s">
+      <c r="C44" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D44" s="171"/>
+      <c r="D44" s="169"/>
       <c r="E44" s="132"/>
       <c r="F44" s="132"/>
       <c r="G44" s="132"/>
-      <c r="H44" s="172"/>
+      <c r="H44" s="170"/>
       <c r="I44" s="132"/>
       <c r="J44" s="132"/>
       <c r="K44" s="132"/>
@@ -7791,18 +7790,18 @@
       <c r="M44" s="132"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A45" s="289"/>
-      <c r="B45" s="153" t="s">
+      <c r="A45" s="284"/>
+      <c r="B45" s="152" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="170" t="s">
+      <c r="C45" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D45" s="171"/>
+      <c r="D45" s="169"/>
       <c r="E45" s="132"/>
       <c r="F45" s="132"/>
       <c r="G45" s="132"/>
-      <c r="H45" s="172"/>
+      <c r="H45" s="170"/>
       <c r="I45" s="132"/>
       <c r="J45" s="132"/>
       <c r="K45" s="132"/>
@@ -7833,8 +7832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7884,10 +7883,10 @@
       <c r="H6" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="252" t="s">
+      <c r="A8" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="247"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -7904,10 +7903,10 @@
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="254" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="259"/>
+      <c r="B10" s="254"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -7947,7 +7946,7 @@
       <c r="M12" s="53"/>
     </row>
     <row r="13" spans="1:13" ht="90" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="260" t="s">
+      <c r="A13" s="255" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -7957,36 +7956,36 @@
         <v>214</v>
       </c>
       <c r="D13" s="55"/>
-      <c r="E13" s="212" t="s">
+      <c r="E13" s="207" t="s">
         <v>347</v>
       </c>
-      <c r="F13" s="213" t="s">
+      <c r="F13" s="208" t="s">
         <v>348</v>
       </c>
-      <c r="G13" s="213" t="s">
+      <c r="G13" s="208" t="s">
         <v>349</v>
       </c>
-      <c r="H13" s="213" t="s">
+      <c r="H13" s="208" t="s">
         <v>350</v>
       </c>
-      <c r="I13" s="213" t="s">
+      <c r="I13" s="208" t="s">
         <v>351</v>
       </c>
-      <c r="J13" s="213" t="s">
+      <c r="J13" s="208" t="s">
         <v>352</v>
       </c>
-      <c r="K13" s="207"/>
+      <c r="K13" s="202"/>
       <c r="L13" s="45"/>
       <c r="M13" s="120"/>
     </row>
     <row r="14" spans="1:13" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="250"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="46"/>
       <c r="D14" s="55"/>
-      <c r="E14" s="211" t="s">
+      <c r="E14" s="206" t="s">
         <v>185</v>
       </c>
       <c r="F14" s="137" t="s">
@@ -8003,7 +8002,7 @@
       <c r="M14" s="121"/>
     </row>
     <row r="15" spans="1:13" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="253" t="s">
+      <c r="A15" s="248" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -8011,32 +8010,32 @@
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="55"/>
-      <c r="E15" s="212" t="s">
+      <c r="E15" s="207" t="s">
         <v>354</v>
       </c>
-      <c r="F15" s="213" t="s">
+      <c r="F15" s="208" t="s">
         <v>355</v>
       </c>
-      <c r="G15" s="213" t="s">
+      <c r="G15" s="208" t="s">
         <v>356</v>
       </c>
-      <c r="H15" s="213" t="s">
+      <c r="H15" s="208" t="s">
         <v>357</v>
       </c>
-      <c r="I15" s="213"/>
-      <c r="J15" s="213"/>
-      <c r="K15" s="213"/>
+      <c r="I15" s="208"/>
+      <c r="J15" s="208"/>
+      <c r="K15" s="208"/>
       <c r="L15" s="45"/>
       <c r="M15" s="120"/>
     </row>
     <row r="16" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="257"/>
+      <c r="A16" s="252"/>
       <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="55"/>
-      <c r="E16" s="211" t="s">
+      <c r="E16" s="206" t="s">
         <v>123</v>
       </c>
       <c r="F16" s="137" t="s">
@@ -8049,33 +8048,33 @@
         <v>357</v>
       </c>
       <c r="I16" s="137"/>
-      <c r="J16" s="210"/>
-      <c r="K16" s="210"/>
+      <c r="J16" s="205"/>
+      <c r="K16" s="205"/>
       <c r="L16" s="49"/>
       <c r="M16" s="124"/>
     </row>
     <row r="17" spans="1:33" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="254"/>
+      <c r="A17" s="249"/>
       <c r="B17" s="36" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="55"/>
-      <c r="E17" s="208" t="s">
+      <c r="E17" s="203" t="s">
         <v>358</v>
       </c>
-      <c r="F17" s="209" t="s">
+      <c r="F17" s="204" t="s">
         <v>359</v>
       </c>
-      <c r="G17" s="214"/>
-      <c r="H17" s="215"/>
-      <c r="I17" s="216"/>
+      <c r="G17" s="209"/>
+      <c r="H17" s="210"/>
+      <c r="I17" s="211"/>
       <c r="J17" s="137"/>
       <c r="K17" s="137"/>
       <c r="L17" s="46"/>
       <c r="M17" s="121"/>
     </row>
     <row r="18" spans="1:33" ht="64.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="256" t="s">
+      <c r="A18" s="251" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="38" t="s">
@@ -8085,30 +8084,30 @@
         <v>223</v>
       </c>
       <c r="D18" s="55"/>
-      <c r="E18" s="217" t="s">
+      <c r="E18" s="212" t="s">
         <v>360</v>
       </c>
-      <c r="F18" s="213" t="s">
+      <c r="F18" s="208" t="s">
         <v>389</v>
       </c>
-      <c r="G18" s="218" t="s">
+      <c r="G18" s="213" t="s">
         <v>361</v>
       </c>
-      <c r="H18" s="218"/>
-      <c r="I18" s="218"/>
-      <c r="J18" s="218"/>
-      <c r="K18" s="218"/>
+      <c r="H18" s="213"/>
+      <c r="I18" s="213"/>
+      <c r="J18" s="213"/>
+      <c r="K18" s="213"/>
       <c r="L18" s="47"/>
       <c r="M18" s="122"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="254"/>
+      <c r="A19" s="249"/>
       <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="55"/>
-      <c r="E19" s="211"/>
+      <c r="E19" s="206"/>
       <c r="F19" s="137"/>
       <c r="G19" s="137"/>
       <c r="H19" s="137"/>
@@ -8119,24 +8118,24 @@
       <c r="M19" s="121"/>
     </row>
     <row r="20" spans="1:33" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="255"/>
+      <c r="A20" s="250"/>
       <c r="B20" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="48"/>
       <c r="D20" s="55"/>
-      <c r="E20" s="219"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
-      <c r="J20" s="220"/>
-      <c r="K20" s="220"/>
+      <c r="E20" s="214"/>
+      <c r="F20" s="215"/>
+      <c r="G20" s="215"/>
+      <c r="H20" s="215"/>
+      <c r="I20" s="215"/>
+      <c r="J20" s="215"/>
+      <c r="K20" s="215"/>
       <c r="L20" s="48"/>
       <c r="M20" s="123"/>
     </row>
     <row r="21" spans="1:33" ht="159.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="290" t="s">
+      <c r="A21" s="285" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="30" t="s">
@@ -8144,32 +8143,32 @@
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="55"/>
-      <c r="E21" s="221" t="s">
+      <c r="E21" s="216" t="s">
         <v>362</v>
       </c>
-      <c r="F21" s="210" t="s">
+      <c r="F21" s="205" t="s">
         <v>363</v>
       </c>
-      <c r="G21" s="210" t="s">
+      <c r="G21" s="205" t="s">
         <v>364</v>
       </c>
-      <c r="H21" s="210" t="s">
+      <c r="H21" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="I21" s="210" t="s">
+      <c r="I21" s="205" t="s">
         <v>365</v>
       </c>
-      <c r="J21" s="223" t="s">
+      <c r="J21" s="218" t="s">
         <v>366</v>
       </c>
-      <c r="K21" s="210" t="s">
+      <c r="K21" s="205" t="s">
         <v>367</v>
       </c>
       <c r="L21" s="49"/>
       <c r="M21" s="124"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A22" s="291"/>
+      <c r="A22" s="286"/>
       <c r="B22" s="10" t="s">
         <v>172</v>
       </c>
@@ -8177,7 +8176,7 @@
         <v>226</v>
       </c>
       <c r="D22" s="55"/>
-      <c r="E22" s="211" t="s">
+      <c r="E22" s="206" t="s">
         <v>224</v>
       </c>
       <c r="F22" s="137" t="s">
@@ -8196,7 +8195,7 @@
       <c r="M22" s="121"/>
     </row>
     <row r="23" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="291"/>
+      <c r="A23" s="286"/>
       <c r="B23" s="10" t="s">
         <v>196</v>
       </c>
@@ -8227,7 +8226,7 @@
       <c r="M23" s="121"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A24" s="291"/>
+      <c r="A24" s="286"/>
       <c r="B24" s="10" t="s">
         <v>197</v>
       </c>
@@ -8246,7 +8245,7 @@
       <c r="M24" s="121"/>
     </row>
     <row r="25" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="291"/>
+      <c r="A25" s="286"/>
       <c r="B25" s="63" t="s">
         <v>170</v>
       </c>
@@ -8269,7 +8268,7 @@
       <c r="M25" s="125"/>
     </row>
     <row r="26" spans="1:33" ht="258" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="292"/>
+      <c r="A26" s="287"/>
       <c r="B26" s="36" t="s">
         <v>18</v>
       </c>
@@ -8289,7 +8288,7 @@
       <c r="H26" s="48" t="s">
         <v>371</v>
       </c>
-      <c r="I26" s="248" t="s">
+      <c r="I26" s="243" t="s">
         <v>357</v>
       </c>
       <c r="J26" s="48"/>
@@ -8336,7 +8335,7 @@
       <c r="M27" s="130"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A28" s="245"/>
+      <c r="A28" s="240"/>
       <c r="B28" s="30" t="s">
         <v>399</v>
       </c>
@@ -8360,10 +8359,10 @@
       <c r="J28" s="10"/>
       <c r="K28" s="99"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="246"/>
+      <c r="M28" s="241"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A29" s="245"/>
+      <c r="A29" s="240"/>
       <c r="B29" s="30" t="s">
         <v>400</v>
       </c>
@@ -8387,10 +8386,10 @@
       <c r="J29" s="10"/>
       <c r="K29" s="99"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="246"/>
+      <c r="M29" s="241"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A30" s="245"/>
+      <c r="A30" s="240"/>
       <c r="B30" s="30" t="s">
         <v>414</v>
       </c>
@@ -8399,14 +8398,14 @@
       <c r="E30" s="99" t="s">
         <v>404</v>
       </c>
-      <c r="F30" s="246"/>
+      <c r="F30" s="241"/>
       <c r="G30" s="99"/>
       <c r="H30" s="30"/>
       <c r="I30" s="102"/>
       <c r="J30" s="30"/>
       <c r="K30" s="102"/>
       <c r="L30" s="30"/>
-      <c r="M30" s="247"/>
+      <c r="M30" s="242"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="107"/>
@@ -8424,7 +8423,7 @@
       <c r="M31" s="127"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A32" s="257" t="s">
+      <c r="A32" s="252" t="s">
         <v>203</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -8469,7 +8468,7 @@
       <c r="W32" s="9"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="254"/>
+      <c r="A33" s="249"/>
       <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
@@ -8526,7 +8525,7 @@
       <c r="W33" s="9"/>
     </row>
     <row r="34" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="258"/>
+      <c r="A34" s="253"/>
       <c r="B34" s="41" t="s">
         <v>48</v>
       </c>
@@ -8578,7 +8577,7 @@
       <c r="G35" s="111" t="s">
         <v>334</v>
       </c>
-      <c r="H35" s="224" t="s">
+      <c r="H35" s="219" t="s">
         <v>376</v>
       </c>
       <c r="I35" s="111"/>
@@ -8638,7 +8637,7 @@
         <v>249</v>
       </c>
       <c r="C37" s="48"/>
-      <c r="D37" s="176"/>
+      <c r="D37" s="174"/>
       <c r="E37" s="131" t="s">
         <v>380</v>
       </c>
@@ -8664,14 +8663,14 @@
       <c r="W37" s="9"/>
     </row>
     <row r="38" spans="1:23" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="288" t="s">
+      <c r="A38" s="283" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="198" t="s">
+      <c r="B38" s="194" t="s">
         <v>262</v>
       </c>
       <c r="C38" s="30"/>
-      <c r="D38" s="174"/>
+      <c r="D38" s="172"/>
       <c r="E38" s="30" t="s">
         <v>382</v>
       </c>
@@ -8681,18 +8680,18 @@
       <c r="G38" s="30"/>
       <c r="H38" s="30"/>
       <c r="I38" s="30"/>
-      <c r="J38" s="173"/>
-      <c r="K38" s="175"/>
-      <c r="L38" s="175"/>
-      <c r="M38" s="175"/>
+      <c r="J38" s="171"/>
+      <c r="K38" s="173"/>
+      <c r="L38" s="173"/>
+      <c r="M38" s="173"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A39" s="289"/>
-      <c r="B39" s="188" t="s">
+      <c r="A39" s="284"/>
+      <c r="B39" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="C39" s="193"/>
-      <c r="D39" s="199"/>
+      <c r="C39" s="191"/>
+      <c r="D39" s="195"/>
       <c r="E39" s="10" t="s">
         <v>347</v>
       </c>
@@ -8708,37 +8707,37 @@
       <c r="I39" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="J39" s="169"/>
+      <c r="J39" s="167"/>
       <c r="K39" s="132"/>
       <c r="L39" s="132"/>
       <c r="M39" s="132"/>
     </row>
     <row r="40" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="289"/>
-      <c r="B40" s="188" t="s">
+      <c r="A40" s="284"/>
+      <c r="B40" s="186" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="193"/>
-      <c r="D40" s="199"/>
-      <c r="E40" s="222" t="s">
+      <c r="C40" s="191"/>
+      <c r="D40" s="195"/>
+      <c r="E40" s="217" t="s">
         <v>386</v>
       </c>
-      <c r="F40" s="193"/>
-      <c r="G40" s="193"/>
-      <c r="H40" s="200"/>
-      <c r="I40" s="193"/>
+      <c r="F40" s="191"/>
+      <c r="G40" s="191"/>
+      <c r="H40" s="196"/>
+      <c r="I40" s="191"/>
       <c r="J40" s="132"/>
       <c r="K40" s="132"/>
       <c r="L40" s="132"/>
       <c r="M40" s="132"/>
     </row>
     <row r="41" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="289"/>
-      <c r="B41" s="188" t="s">
+      <c r="A41" s="284"/>
+      <c r="B41" s="186" t="s">
         <v>277</v>
       </c>
-      <c r="C41" s="193"/>
-      <c r="D41" s="199"/>
+      <c r="C41" s="191"/>
+      <c r="D41" s="195"/>
       <c r="E41" s="10" t="s">
         <v>374</v>
       </c>
@@ -8758,18 +8757,18 @@
       <c r="M41" s="132"/>
     </row>
     <row r="42" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="289"/>
-      <c r="B42" s="153" t="s">
+      <c r="A42" s="284"/>
+      <c r="B42" s="152" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="170" t="s">
+      <c r="C42" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D42" s="171"/>
+      <c r="D42" s="169"/>
       <c r="E42" s="132"/>
       <c r="F42" s="132"/>
       <c r="G42" s="132"/>
-      <c r="H42" s="172"/>
+      <c r="H42" s="170"/>
       <c r="I42" s="132"/>
       <c r="J42" s="132"/>
       <c r="K42" s="132"/>
@@ -8777,18 +8776,18 @@
       <c r="M42" s="132"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A43" s="289"/>
-      <c r="B43" s="153" t="s">
+      <c r="A43" s="284"/>
+      <c r="B43" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="170" t="s">
+      <c r="C43" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D43" s="171"/>
+      <c r="D43" s="169"/>
       <c r="E43" s="132"/>
       <c r="F43" s="132"/>
       <c r="G43" s="132"/>
-      <c r="H43" s="172"/>
+      <c r="H43" s="170"/>
       <c r="I43" s="132"/>
       <c r="J43" s="132"/>
       <c r="K43" s="132"/>
@@ -8796,18 +8795,18 @@
       <c r="M43" s="132"/>
     </row>
     <row r="44" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="289"/>
-      <c r="B44" s="153" t="s">
+      <c r="A44" s="284"/>
+      <c r="B44" s="152" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="170" t="s">
+      <c r="C44" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D44" s="171"/>
+      <c r="D44" s="169"/>
       <c r="E44" s="132"/>
       <c r="F44" s="132"/>
       <c r="G44" s="132"/>
-      <c r="H44" s="172"/>
+      <c r="H44" s="170"/>
       <c r="I44" s="132"/>
       <c r="J44" s="132"/>
       <c r="K44" s="132"/>
@@ -8815,18 +8814,18 @@
       <c r="M44" s="132"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A45" s="289"/>
-      <c r="B45" s="153" t="s">
+      <c r="A45" s="284"/>
+      <c r="B45" s="152" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="170" t="s">
+      <c r="C45" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D45" s="171"/>
+      <c r="D45" s="169"/>
       <c r="E45" s="132"/>
       <c r="F45" s="132"/>
       <c r="G45" s="132"/>
-      <c r="H45" s="172"/>
+      <c r="H45" s="170"/>
       <c r="I45" s="132"/>
       <c r="J45" s="132"/>
       <c r="K45" s="132"/>
@@ -8906,10 +8905,10 @@
       <c r="H6" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="252" t="s">
+      <c r="A8" s="247" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="252"/>
+      <c r="B8" s="247"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -8926,10 +8925,10 @@
       <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="254" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="259"/>
+      <c r="B10" s="254"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
@@ -8969,7 +8968,7 @@
       <c r="M12" s="53"/>
     </row>
     <row r="13" spans="1:13" ht="90" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="260" t="s">
+      <c r="A13" s="255" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -8997,18 +8996,18 @@
       <c r="J13" s="45" t="s">
         <v>303</v>
       </c>
-      <c r="K13" s="207"/>
+      <c r="K13" s="202"/>
       <c r="L13" s="45"/>
       <c r="M13" s="120"/>
     </row>
     <row r="14" spans="1:13" ht="12.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="250"/>
+      <c r="A14" s="245"/>
       <c r="B14" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="46"/>
       <c r="D14" s="55"/>
-      <c r="E14" s="211" t="s">
+      <c r="E14" s="206" t="s">
         <v>185</v>
       </c>
       <c r="F14" s="137" t="s">
@@ -9025,7 +9024,7 @@
       <c r="M14" s="121"/>
     </row>
     <row r="15" spans="1:13" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="253" t="s">
+      <c r="A15" s="248" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -9033,32 +9032,32 @@
       </c>
       <c r="C15" s="45"/>
       <c r="D15" s="55"/>
-      <c r="E15" s="212" t="s">
+      <c r="E15" s="207" t="s">
         <v>307</v>
       </c>
-      <c r="F15" s="213" t="s">
+      <c r="F15" s="208" t="s">
         <v>308</v>
       </c>
-      <c r="G15" s="213" t="s">
+      <c r="G15" s="208" t="s">
         <v>309</v>
       </c>
-      <c r="H15" s="213" t="s">
+      <c r="H15" s="208" t="s">
         <v>310</v>
       </c>
-      <c r="I15" s="213"/>
+      <c r="I15" s="208"/>
       <c r="J15" s="45"/>
       <c r="K15" s="45"/>
       <c r="L15" s="45"/>
       <c r="M15" s="120"/>
     </row>
     <row r="16" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="257"/>
+      <c r="A16" s="252"/>
       <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="46"/>
       <c r="D16" s="55"/>
-      <c r="E16" s="211" t="s">
+      <c r="E16" s="206" t="s">
         <v>311</v>
       </c>
       <c r="F16" s="137" t="s">
@@ -9077,27 +9076,27 @@
       <c r="M16" s="124"/>
     </row>
     <row r="17" spans="1:33" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="254"/>
+      <c r="A17" s="249"/>
       <c r="B17" s="36" t="s">
         <v>13</v>
       </c>
       <c r="D17" s="55"/>
-      <c r="E17" s="208" t="s">
+      <c r="E17" s="203" t="s">
         <v>314</v>
       </c>
-      <c r="F17" s="209" t="s">
+      <c r="F17" s="204" t="s">
         <v>315</v>
       </c>
-      <c r="G17" s="214"/>
-      <c r="H17" s="215"/>
-      <c r="I17" s="216"/>
+      <c r="G17" s="209"/>
+      <c r="H17" s="210"/>
+      <c r="I17" s="211"/>
       <c r="J17" s="46"/>
       <c r="K17" s="46"/>
       <c r="L17" s="46"/>
       <c r="M17" s="121"/>
     </row>
     <row r="18" spans="1:33" ht="64.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="256" t="s">
+      <c r="A18" s="251" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="38" t="s">
@@ -9107,30 +9106,30 @@
         <v>223</v>
       </c>
       <c r="D18" s="55"/>
-      <c r="E18" s="217" t="s">
+      <c r="E18" s="212" t="s">
         <v>316</v>
       </c>
-      <c r="F18" s="218" t="s">
+      <c r="F18" s="213" t="s">
         <v>390</v>
       </c>
-      <c r="G18" s="218" t="s">
+      <c r="G18" s="213" t="s">
         <v>317</v>
       </c>
-      <c r="H18" s="218"/>
-      <c r="I18" s="218"/>
+      <c r="H18" s="213"/>
+      <c r="I18" s="213"/>
       <c r="J18" s="47"/>
       <c r="K18" s="47"/>
       <c r="L18" s="47"/>
       <c r="M18" s="122"/>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A19" s="254"/>
+      <c r="A19" s="249"/>
       <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="46"/>
       <c r="D19" s="55"/>
-      <c r="E19" s="211"/>
+      <c r="E19" s="206"/>
       <c r="F19" s="137"/>
       <c r="G19" s="137"/>
       <c r="H19" s="137"/>
@@ -9141,24 +9140,24 @@
       <c r="M19" s="121"/>
     </row>
     <row r="20" spans="1:33" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="255"/>
+      <c r="A20" s="250"/>
       <c r="B20" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="48"/>
       <c r="D20" s="55"/>
-      <c r="E20" s="219"/>
-      <c r="F20" s="220"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="220"/>
+      <c r="E20" s="214"/>
+      <c r="F20" s="215"/>
+      <c r="G20" s="215"/>
+      <c r="H20" s="215"/>
+      <c r="I20" s="215"/>
       <c r="J20" s="48"/>
       <c r="K20" s="48"/>
       <c r="L20" s="48"/>
       <c r="M20" s="123"/>
     </row>
     <row r="21" spans="1:33" ht="159.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="290" t="s">
+      <c r="A21" s="285" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="30" t="s">
@@ -9166,22 +9165,22 @@
       </c>
       <c r="C21" s="49"/>
       <c r="D21" s="55"/>
-      <c r="E21" s="221" t="s">
+      <c r="E21" s="216" t="s">
         <v>318</v>
       </c>
-      <c r="F21" s="210" t="s">
+      <c r="F21" s="205" t="s">
         <v>319</v>
       </c>
-      <c r="G21" s="210" t="s">
+      <c r="G21" s="205" t="s">
         <v>320</v>
       </c>
-      <c r="H21" s="210" t="s">
+      <c r="H21" s="205" t="s">
         <v>130</v>
       </c>
-      <c r="I21" s="210" t="s">
+      <c r="I21" s="205" t="s">
         <v>321</v>
       </c>
-      <c r="J21" s="204" t="s">
+      <c r="J21" s="199" t="s">
         <v>322</v>
       </c>
       <c r="K21" s="49" t="s">
@@ -9191,7 +9190,7 @@
       <c r="M21" s="124"/>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A22" s="291"/>
+      <c r="A22" s="286"/>
       <c r="B22" s="10" t="s">
         <v>172</v>
       </c>
@@ -9199,7 +9198,7 @@
         <v>226</v>
       </c>
       <c r="D22" s="55"/>
-      <c r="E22" s="211" t="s">
+      <c r="E22" s="206" t="s">
         <v>224</v>
       </c>
       <c r="F22" s="137" t="s">
@@ -9218,7 +9217,7 @@
       <c r="M22" s="121"/>
     </row>
     <row r="23" spans="1:33" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="291"/>
+      <c r="A23" s="286"/>
       <c r="B23" s="10" t="s">
         <v>196</v>
       </c>
@@ -9226,7 +9225,7 @@
         <v>227</v>
       </c>
       <c r="D23" s="55"/>
-      <c r="E23" s="211" t="s">
+      <c r="E23" s="206" t="s">
         <v>163</v>
       </c>
       <c r="F23" s="137" t="s">
@@ -9249,7 +9248,7 @@
       <c r="M23" s="121"/>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A24" s="291"/>
+      <c r="A24" s="286"/>
       <c r="B24" s="10" t="s">
         <v>197</v>
       </c>
@@ -9268,7 +9267,7 @@
       <c r="M24" s="121"/>
     </row>
     <row r="25" spans="1:33" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="291"/>
+      <c r="A25" s="286"/>
       <c r="B25" s="63" t="s">
         <v>170</v>
       </c>
@@ -9291,7 +9290,7 @@
       <c r="M25" s="125"/>
     </row>
     <row r="26" spans="1:33" ht="258" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="292"/>
+      <c r="A26" s="287"/>
       <c r="B26" s="36" t="s">
         <v>18</v>
       </c>
@@ -9311,7 +9310,7 @@
       <c r="H26" s="48" t="s">
         <v>325</v>
       </c>
-      <c r="I26" s="248" t="s">
+      <c r="I26" s="243" t="s">
         <v>310</v>
       </c>
       <c r="J26" s="48"/>
@@ -9358,7 +9357,7 @@
       <c r="M27" s="130"/>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A28" s="245"/>
+      <c r="A28" s="240"/>
       <c r="B28" s="30" t="s">
         <v>399</v>
       </c>
@@ -9382,10 +9381,10 @@
       <c r="J28" s="10"/>
       <c r="K28" s="99"/>
       <c r="L28" s="10"/>
-      <c r="M28" s="246"/>
+      <c r="M28" s="241"/>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A29" s="245"/>
+      <c r="A29" s="240"/>
       <c r="B29" s="30" t="s">
         <v>400</v>
       </c>
@@ -9409,10 +9408,10 @@
       <c r="J29" s="10"/>
       <c r="K29" s="99"/>
       <c r="L29" s="10"/>
-      <c r="M29" s="246"/>
+      <c r="M29" s="241"/>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A30" s="245"/>
+      <c r="A30" s="240"/>
       <c r="B30" s="30" t="s">
         <v>414</v>
       </c>
@@ -9421,14 +9420,14 @@
       <c r="E30" s="99" t="s">
         <v>420</v>
       </c>
-      <c r="F30" s="246"/>
+      <c r="F30" s="241"/>
       <c r="G30" s="99"/>
       <c r="H30" s="30"/>
       <c r="I30" s="102"/>
       <c r="J30" s="30"/>
       <c r="K30" s="102"/>
       <c r="L30" s="30"/>
-      <c r="M30" s="247"/>
+      <c r="M30" s="242"/>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A31" s="107"/>
@@ -9446,7 +9445,7 @@
       <c r="M31" s="127"/>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A32" s="257" t="s">
+      <c r="A32" s="252" t="s">
         <v>203</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -9491,7 +9490,7 @@
       <c r="W32" s="9"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="254"/>
+      <c r="A33" s="249"/>
       <c r="B33" s="10" t="s">
         <v>46</v>
       </c>
@@ -9548,7 +9547,7 @@
       <c r="W33" s="9"/>
     </row>
     <row r="34" spans="1:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="258"/>
+      <c r="A34" s="253"/>
       <c r="B34" s="41" t="s">
         <v>48</v>
       </c>
@@ -9660,7 +9659,7 @@
         <v>249</v>
       </c>
       <c r="C37" s="48"/>
-      <c r="D37" s="176"/>
+      <c r="D37" s="174"/>
       <c r="E37" s="131" t="s">
         <v>339</v>
       </c>
@@ -9686,14 +9685,14 @@
       <c r="W37" s="9"/>
     </row>
     <row r="38" spans="1:23" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="288" t="s">
+      <c r="A38" s="283" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="198" t="s">
+      <c r="B38" s="194" t="s">
         <v>262</v>
       </c>
       <c r="C38" s="30"/>
-      <c r="D38" s="174"/>
+      <c r="D38" s="172"/>
       <c r="E38" s="30" t="s">
         <v>341</v>
       </c>
@@ -9703,18 +9702,18 @@
       <c r="G38" s="30"/>
       <c r="H38" s="30"/>
       <c r="I38" s="30"/>
-      <c r="J38" s="173"/>
-      <c r="K38" s="175"/>
-      <c r="L38" s="175"/>
-      <c r="M38" s="175"/>
+      <c r="J38" s="171"/>
+      <c r="K38" s="173"/>
+      <c r="L38" s="173"/>
+      <c r="M38" s="173"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A39" s="289"/>
-      <c r="B39" s="188" t="s">
+      <c r="A39" s="284"/>
+      <c r="B39" s="186" t="s">
         <v>283</v>
       </c>
-      <c r="C39" s="193"/>
-      <c r="D39" s="199"/>
+      <c r="C39" s="191"/>
+      <c r="D39" s="195"/>
       <c r="E39" s="10" t="s">
         <v>298</v>
       </c>
@@ -9730,37 +9729,37 @@
       <c r="I39" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="J39" s="169"/>
+      <c r="J39" s="167"/>
       <c r="K39" s="132"/>
       <c r="L39" s="132"/>
       <c r="M39" s="132"/>
     </row>
     <row r="40" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="289"/>
-      <c r="B40" s="188" t="s">
+      <c r="A40" s="284"/>
+      <c r="B40" s="186" t="s">
         <v>102</v>
       </c>
-      <c r="C40" s="193"/>
-      <c r="D40" s="199"/>
-      <c r="E40" s="222" t="s">
+      <c r="C40" s="191"/>
+      <c r="D40" s="195"/>
+      <c r="E40" s="217" t="s">
         <v>345</v>
       </c>
-      <c r="F40" s="193"/>
-      <c r="G40" s="193"/>
-      <c r="H40" s="200"/>
-      <c r="I40" s="193"/>
+      <c r="F40" s="191"/>
+      <c r="G40" s="191"/>
+      <c r="H40" s="196"/>
+      <c r="I40" s="191"/>
       <c r="J40" s="132"/>
       <c r="K40" s="132"/>
       <c r="L40" s="132"/>
       <c r="M40" s="132"/>
     </row>
     <row r="41" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="289"/>
-      <c r="B41" s="188" t="s">
+      <c r="A41" s="284"/>
+      <c r="B41" s="186" t="s">
         <v>277</v>
       </c>
-      <c r="C41" s="193"/>
-      <c r="D41" s="199"/>
+      <c r="C41" s="191"/>
+      <c r="D41" s="195"/>
       <c r="E41" s="10" t="s">
         <v>346</v>
       </c>
@@ -9780,18 +9779,18 @@
       <c r="M41" s="132"/>
     </row>
     <row r="42" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="289"/>
-      <c r="B42" s="153" t="s">
+      <c r="A42" s="284"/>
+      <c r="B42" s="152" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="170" t="s">
+      <c r="C42" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D42" s="171"/>
+      <c r="D42" s="169"/>
       <c r="E42" s="132"/>
       <c r="F42" s="132"/>
       <c r="G42" s="132"/>
-      <c r="H42" s="172"/>
+      <c r="H42" s="170"/>
       <c r="I42" s="132"/>
       <c r="J42" s="132"/>
       <c r="K42" s="132"/>
@@ -9799,18 +9798,18 @@
       <c r="M42" s="132"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A43" s="289"/>
-      <c r="B43" s="153" t="s">
+      <c r="A43" s="284"/>
+      <c r="B43" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="C43" s="170" t="s">
+      <c r="C43" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D43" s="171"/>
+      <c r="D43" s="169"/>
       <c r="E43" s="132"/>
       <c r="F43" s="132"/>
       <c r="G43" s="132"/>
-      <c r="H43" s="172"/>
+      <c r="H43" s="170"/>
       <c r="I43" s="132"/>
       <c r="J43" s="132"/>
       <c r="K43" s="132"/>
@@ -9818,18 +9817,18 @@
       <c r="M43" s="132"/>
     </row>
     <row r="44" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="289"/>
-      <c r="B44" s="153" t="s">
+      <c r="A44" s="284"/>
+      <c r="B44" s="152" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="170" t="s">
+      <c r="C44" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D44" s="171"/>
+      <c r="D44" s="169"/>
       <c r="E44" s="132"/>
       <c r="F44" s="132"/>
       <c r="G44" s="132"/>
-      <c r="H44" s="172"/>
+      <c r="H44" s="170"/>
       <c r="I44" s="132"/>
       <c r="J44" s="132"/>
       <c r="K44" s="132"/>
@@ -9837,18 +9836,18 @@
       <c r="M44" s="132"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A45" s="289"/>
-      <c r="B45" s="153" t="s">
+      <c r="A45" s="284"/>
+      <c r="B45" s="152" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="170" t="s">
+      <c r="C45" s="168" t="s">
         <v>285</v>
       </c>
-      <c r="D45" s="171"/>
+      <c r="D45" s="169"/>
       <c r="E45" s="132"/>
       <c r="F45" s="132"/>
       <c r="G45" s="132"/>
-      <c r="H45" s="172"/>
+      <c r="H45" s="170"/>
       <c r="I45" s="132"/>
       <c r="J45" s="132"/>
       <c r="K45" s="132"/>

</xml_diff>